<commit_message>
submitted before ded is finished!
</commit_message>
<xml_diff>
--- a/EOBReceiveFeesFromCigna/EOB.xlsx
+++ b/EOBReceiveFeesFromCigna/EOB.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,47 +424,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>'U71369331</t>
+          <t>'U56733636</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>'4682312813839</t>
+          <t>'9652408096438</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>LI</t>
+          <t>LIAO</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>XINRAN</t>
+          <t>YONGXIANG</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>02/10/2023</t>
+          <t>12/11/2023</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>900.00</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>201.23</t>
+          <t>240.00</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>395.00</t>
+          <t>416.70</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -507,47 +507,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>'U71369331</t>
+          <t>'U56733636</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>'4682312813840</t>
+          <t>'9652408096440</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>LI</t>
+          <t>LIAO</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>XINRAN</t>
+          <t>YONGXIANG</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>02/15/2023</t>
+          <t>11/13/2023</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>900.00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>201.23</t>
+          <t>319.81</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>395.00</t>
+          <t>416.70</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -590,47 +590,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>'U71369331</t>
+          <t>'U56733636</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>'4682312813850</t>
+          <t>'9652408096441</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>LI</t>
+          <t>LIAO</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>XINRAN</t>
+          <t>YONGXIANG</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>01/30/2023</t>
+          <t>11/29/2023</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>900.00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>201.23</t>
+          <t>319.81</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>395.00</t>
+          <t>416.70</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -673,47 +673,47 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>'U71369331</t>
+          <t>'U56733636</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>'4682312813852</t>
+          <t>'9652408096443</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LI</t>
+          <t>LIAO</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>XINRAN</t>
+          <t>YONGXIANG</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>02/17/2023</t>
+          <t>12/07/2023</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>900.00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>201.23</t>
+          <t>319.81</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>395.00</t>
+          <t>416.70</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -756,47 +756,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>'U71369331</t>
+          <t>'U56733636</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>'4682312813853</t>
+          <t>'9652408096663</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>LI</t>
+          <t>LIAO</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>XINRAN</t>
+          <t>YONGXIANG</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>02/24/2023</t>
+          <t>11/20/2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>900.00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>201.23</t>
+          <t>319.81</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>395.00</t>
+          <t>416.70</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -839,47 +839,47 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>'U71369331</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>'4682312813857</t>
+          <t>'4682412800131</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>LI</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>XINRAN</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>02/22/2023</t>
+          <t>02/14/2024</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>201.23</t>
+          <t>65.03</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>395.00</t>
+          <t>92.90</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -922,47 +922,47 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>'U71369331</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>'4682312813858</t>
+          <t>'4682412800132</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>LI</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>XINRAN</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>02/08/2023</t>
+          <t>02/28/2024</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>201.23</t>
+          <t>65.03</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>395.00</t>
+          <t>92.90</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1005,47 +1005,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>'U71369331</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>'4682312813859</t>
+          <t>'4682412800133</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>LI</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>XINRAN</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>02/01/2023</t>
+          <t>03/06/2024</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>201.23</t>
+          <t>65.03</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>395.00</t>
+          <t>92.90</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1088,47 +1088,47 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>'U68421583</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>'7682311615410</t>
+          <t>'4682412800134</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>'230831090004334</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PANDAY</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>NABINA</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>02/08/2023</t>
+          <t>03/27/2024</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>900.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>226.07</t>
+          <t>66.12</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>355.25</t>
+          <t>94.46</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1171,52 +1171,64 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>'106945895</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>'232588119900</t>
+          <t>'4682412800135</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>'603600789007</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>DISANZA</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CHRISTINA</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>07/03/23</t>
+          <t>03/13/2024</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>90.42</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
@@ -1242,52 +1254,64 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>'106945895</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>'232588120600</t>
+          <t>'4682412800136</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>'603600789007</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>DISANZA</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CHRISTINA</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>07/07/23</t>
+          <t>04/03/2024</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>90.42</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
@@ -1313,52 +1337,64 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>'106945895</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>'232588121000</t>
+          <t>'4682412800137</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>'603600789007</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>DISANZA</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CHRISTINA</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>07/14/23</t>
+          <t>02/16/2024</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>90.42</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+          <t>65.03</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>92.90</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
@@ -1384,52 +1420,64 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>'106945895</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>'232588120200</t>
+          <t>'4682412800138</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>'603600789007</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>DISANZA</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CHRISTINA</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>07/21/23</t>
+          <t>02/21/2024</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>90.42</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+          <t>65.03</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>92.90</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
@@ -1455,52 +1503,64 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>'106945895</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>'232588122400</t>
+          <t>'4682412800139</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>'603600789007</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>DISANZA</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CHRISTINA</t>
+          <t>ELENI</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>08/15/23</t>
+          <t>03/20/2024</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>90.42</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
@@ -1526,48 +1586,64 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>'106945895</t>
+          <t>'U91200304</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>'232588119500</t>
+          <t>'4682412800140</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>'603600789007</t>
+          <t>'240516090004339</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>DISANZA</t>
+          <t>SALTOS</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>CHRISTINA</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
+          <t>ELENI</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>04/10/2024</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>760.00</t>
+          <t>800.00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>90.42</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
@@ -1585,140 +1661,6 @@
         </is>
       </c>
       <c r="Q15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>'106945895</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>'232588122800</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>'603600789007</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>DISANZA</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>CHRISTINA</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>760.00</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>90.42</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>'106945895</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>'232588119300</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>'603600789007</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>DISANZA</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>CHRISTINA</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>760.00</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>90.42</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
         <is>
           <t>NO</t>
         </is>

</xml_diff>

<commit_message>
submitted before None is removed!
</commit_message>
<xml_diff>
--- a/EOBReceiveFeesFromCigna/EOB.xlsx
+++ b/EOBReceiveFeesFromCigna/EOB.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,47 +424,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>'U56733636</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>'9652408096438</t>
+          <t>'4682415012033</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>LIAO</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>YONGXIANG</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>12/11/2023</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>900.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>240.00</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>416.70</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -505,56 +505,24 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>'U56733636</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>'9652408096440</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>LIAO</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>YONGXIANG</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>11/13/2023</t>
-        </is>
-      </c>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>900.00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>319.81</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>416.70</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>0.0</t>
@@ -590,47 +558,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>'U56733636</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>'9652408096441</t>
+          <t>'4682415012034</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>LIAO</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>YONGXIANG</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>11/29/2023</t>
+          <t>01/12/2024</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>900.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>319.81</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>416.70</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -673,52 +641,52 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>'U56733636</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>'9652408096443</t>
+          <t>'4682415012035</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LIAO</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>YONGXIANG</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>01/15/2024</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>900.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>319.81</t>
+          <t>122.18</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>416.70</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>331.72</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -756,47 +724,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>'U56733636</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>'9652408096663</t>
+          <t>'4682415012037</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>LIAO</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>YONGXIANG</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11/20/2023</t>
+          <t>01/19/2024</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>900.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>319.81</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>416.70</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -839,47 +807,47 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>'4682412800131</t>
+          <t>'4682415012038</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>02/14/2024</t>
+          <t>02/05/2024</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>800.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>65.03</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>92.90</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -922,47 +890,47 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>'4682412800132</t>
+          <t>'4682415012039</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>02/28/2024</t>
+          <t>01/29/2024</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>800.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>65.03</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>92.90</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1005,47 +973,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>'4682412800133</t>
+          <t>'4682417115019</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>03/08/2024</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>800.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>65.03</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>92.90</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1088,47 +1056,47 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>'4682412800134</t>
+          <t>'4682417115020</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>03/27/2024</t>
+          <t>02/23/2024</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>800.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>66.12</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>94.46</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1171,47 +1139,47 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>'4682412800135</t>
+          <t>'4682417115022</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>03/13/2024</t>
+          <t>02/19/2024</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>800.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>66.12</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>94.46</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1254,47 +1222,47 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>'4682412800136</t>
+          <t>'4682417115023</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>04/03/2024</t>
+          <t>02/29/2024</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>800.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>66.12</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>94.46</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1337,47 +1305,47 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U68769899</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>'4682412800137</t>
+          <t>'4682417115211</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>WALL</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>CODY</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>02/16/2024</t>
+          <t>02/26/2024</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>800.00</t>
+          <t>760.00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>65.03</t>
+          <t>387.55</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>92.90</t>
+          <t>484.44</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1420,32 +1388,32 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U49610508</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>'4682412800138</t>
+          <t>'7682419594899</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>NIKA</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>ELIVERTA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>02/21/2024</t>
+          <t>03/01/2024</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1503,32 +1471,32 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U49610508</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>'4682412800139</t>
+          <t>'7682419594900</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>NIKA</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>ELIVERTA</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>03/20/2024</t>
+          <t>03/08/2024</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1538,12 +1506,12 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>66.12</t>
+          <t>65.03</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>94.46</t>
+          <t>92.90</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1586,32 +1554,32 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>'U91200304</t>
+          <t>'U49610508</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>'4682412800140</t>
+          <t>'7682419594901</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>'240516090004339</t>
+          <t>'240816090002811</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>SALTOS</t>
+          <t>NIKA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ELENI</t>
+          <t>ELIVERTA</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>02/23/2024</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1621,12 +1589,12 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>66.12</t>
+          <t>65.03</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>94.46</t>
+          <t>92.90</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1661,6 +1629,753 @@
         </is>
       </c>
       <c r="Q15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>'7682419594902</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>03/18/2024</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>'7682419594903</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>03/27/2024</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>'7682419594904</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>02/28/2024</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>65.03</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>92.90</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>'7682419594905</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>04/01/2024</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>'7682419594906</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>02/21/2024</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>65.03</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>92.90</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>'7682419594907</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>04/08/2024</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>'7682419595466</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>03/06/2024</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>65.03</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>92.90</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>'7682419595467</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>03/13/2024</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>'U49610508</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>'7682419595468</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>'240816090002811</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>NIKA</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>ELIVERTA</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>03/15/2024</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>800.00</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>66.12</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>94.46</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>921279283</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
         <is>
           <t>NO</t>
         </is>

</xml_diff>